<commit_message>
added parallel test methods
</commit_message>
<xml_diff>
--- a/testData/inputSheet.xlsx
+++ b/testData/inputSheet.xlsx
@@ -8,30 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ujjwalsingh\PlayWright-CQA\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2FBDFF-6AE7-497A-BC2F-0EAC8970C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A425EA1-2920-48E5-A30D-29D04EA62DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dcPages1" sheetId="1" r:id="rId1"/>
+    <sheet name="dcPages2" sheetId="2" r:id="rId2"/>
+    <sheet name="dcPages3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>url</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/ar/acrobat/pricing/compare-versions.html</t>
   </si>
   <si>
     <t>https://www.stage.adobe.com/kr/acrobat/pricing/compare-versions.html</t>
   </si>
   <si>
     <t>https://www.stage.adobe.com/tr/acrobat/pricing/compare-versions.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/ar/acrobat/pricing/compare-versions.html</t>
   </si>
 </sst>
 </file>
@@ -69,7 +71,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -97,12 +106,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -415,49 +427,31 @@
   <dimension ref="A1:A88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.69140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5"/>
-    </row>
-    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6"/>
-    </row>
-    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8"/>
-    </row>
-    <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9"/>
-    </row>
+    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="12" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -536,16 +530,67 @@
     <row r="85" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="86" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="87" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="2"/>
+      <c r="A87" s="3"/>
     </row>
     <row r="88" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2"/>
+      <c r="A88" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EB7AC2-4D9C-4E1E-B35E-489B916DA955}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4081A646-3F53-46E7-8A67-D7658901E762}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{C600BDD2-4A7C-42F7-B592-F1F6923184EF}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{78CCABBB-B7AC-41D0-821D-04B45F64FD44}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E5FECBD9-FFE3-48AD-BDD0-52589EED9DE1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060541F5-E805-4846-A20F-B16F50AA258C}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8FA379E4-E3F6-4DC2-B5CB-6B04FCE876A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
developed method for parallel testing and also updated the merchCard and compareCards methods
</commit_message>
<xml_diff>
--- a/testData/inputSheet.xlsx
+++ b/testData/inputSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ujjwalsingh\PlayWright-CQA\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A425EA1-2920-48E5-A30D-29D04EA62DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74436A7-7D7B-4162-A098-C083CD9591FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dcPages1" sheetId="1" r:id="rId1"/>
@@ -27,20 +27,20 @@
     <t>url</t>
   </si>
   <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/pricing/compare-versions.html</t>
-  </si>
-  <si>
     <t>https://www.stage.adobe.com/tr/acrobat/pricing/compare-versions.html</t>
   </si>
   <si>
     <t>https://www.stage.adobe.com/ar/acrobat/pricing/compare-versions.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/pricing/compare-versions.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,14 +54,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -71,7 +63,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -101,10 +93,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -117,10 +123,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,10 +429,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A88"/>
+  <dimension ref="A1:A86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -447,10 +452,18 @@
     </row>
     <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5"/>
+    </row>
+    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6"/>
+    </row>
+    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7"/>
+    </row>
+    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8"/>
+    </row>
     <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -507,34 +520,32 @@
     <row r="62" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="63" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="64" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="67" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="68" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="69" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="70" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="71" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="73" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="75" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="76" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="79" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="80" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="81" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="82" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="3"/>
-    </row>
-    <row r="88" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="3"/>
-    </row>
+    <row r="65" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -542,7 +553,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EB7AC2-4D9C-4E1E-B35E-489B916DA955}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -556,23 +567,38 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E5FECBD9-FFE3-48AD-BDD0-52589EED9DE1}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060541F5-E805-4846-A20F-B16F50AA258C}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -584,14 +610,29 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8FA379E4-E3F6-4DC2-B5CB-6B04FCE876A2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added newContxt method as a common method
</commit_message>
<xml_diff>
--- a/testData/inputSheet.xlsx
+++ b/testData/inputSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ujjwalsingh\PlayWright-CQA\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74436A7-7D7B-4162-A098-C083CD9591FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE942C32-06A4-498B-AC9B-3EA90E092BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dcPages1" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/pricing/compare-versions.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/ar/acrobat/pricing/compare-versions.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/pricing/compare-versions.html</t>
+    <t>https://www.stage.adobe.com/tr/acrobat/pdf-reader.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/tr/acrobat/features.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/tr/acrobat/complete-pdf-solution.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/tr/acrobat/acrobat-standard.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/tr/acrobat/acrobat-pro.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/tr/acrobat.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/pdf-reader.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/features.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/complete-pdf-solution.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/acrobat-standard.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat/acrobat-pro.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/kr/acrobat.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/ar/acrobat/pdf-reader.html</t>
+  </si>
+  <si>
+    <t>https://www.stage.adobe.com/ar/acrobat/generative-ai-pdf/resume-ai.html</t>
   </si>
 </sst>
 </file>
@@ -429,10 +462,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:A85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -447,23 +480,33 @@
     </row>
     <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5"/>
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6"/>
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8"/>
-    </row>
+    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -532,20 +575,19 @@
     <row r="74" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="75" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="76" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="3"/>
+    </row>
     <row r="78" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="3"/>
-    </row>
+    <row r="79" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="80" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="81" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="82" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="83" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="84" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="85" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -553,10 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EB7AC2-4D9C-4E1E-B35E-489B916DA955}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -568,26 +610,31 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -596,10 +643,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060541F5-E805-4846-A20F-B16F50AA258C}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A6:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -611,26 +658,23 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4"/>
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4"/>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added methods to validate acrobat blade and also updated other methods
</commit_message>
<xml_diff>
--- a/testData/inputSheet.xlsx
+++ b/testData/inputSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ujjwalsingh\PlayWright-CQA\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE942C32-06A4-498B-AC9B-3EA90E092BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D6F7F-4034-4C2A-BF7D-51058B3D2BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dcPages1" sheetId="1" r:id="rId1"/>
@@ -22,51 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/pdf-reader.html</t>
+    <t>https://www.stage.adobe.com/in/acrobat/pricing/compare-versions.html</t>
   </si>
   <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/features.html</t>
+    <t>https://www.stage.adobe.com/uk/acrobat/pricing/compare-versions.html</t>
   </si>
   <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/complete-pdf-solution.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/acrobat-standard.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/tr/acrobat/acrobat-pro.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/tr/acrobat.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/pdf-reader.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/features.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/complete-pdf-solution.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/acrobat-standard.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat/acrobat-pro.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/kr/acrobat.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/ar/acrobat/pdf-reader.html</t>
-  </si>
-  <si>
-    <t>https://www.stage.adobe.com/ar/acrobat/generative-ai-pdf/resume-ai.html</t>
+    <t>https://www.stage.adobe.com/hk_en/acrobat/pricing/compare-versions.html</t>
   </si>
 </sst>
 </file>
@@ -96,7 +63,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,41 +78,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -153,10 +90,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,132 +395,519 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A85"/>
+  <dimension ref="A1:A418"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7265625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5"/>
+    </row>
+    <row r="6" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6"/>
+    </row>
+    <row r="7" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="27" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="28" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="29" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="30" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="31" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="50" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="51" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="52" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="53" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="54" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="55" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="57" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="59" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="60" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="62" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="63" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="64" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="67" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="68" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="69" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="71" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="73" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="75" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="76" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="80" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="81" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="82" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8"/>
+    </row>
+    <row r="9" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9"/>
+    </row>
+    <row r="10" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10"/>
+    </row>
+    <row r="11" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11"/>
+    </row>
+    <row r="12" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12"/>
+    </row>
+    <row r="13" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13"/>
+    </row>
+    <row r="14" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14"/>
+    </row>
+    <row r="15" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15"/>
+    </row>
+    <row r="16" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16"/>
+    </row>
+    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17"/>
+    </row>
+    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18"/>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19"/>
+    </row>
+    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20"/>
+    </row>
+    <row r="21" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39"/>
+    </row>
+    <row r="40" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40"/>
+    </row>
+    <row r="41" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41"/>
+    </row>
+    <row r="42" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42"/>
+    </row>
+    <row r="43" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43"/>
+    </row>
+    <row r="44" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44"/>
+    </row>
+    <row r="45" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45"/>
+    </row>
+    <row r="46" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46"/>
+    </row>
+    <row r="47" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47"/>
+    </row>
+    <row r="48" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48"/>
+    </row>
+    <row r="49" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="65" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="66" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="153" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="154" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="155" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="156" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="157" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="158" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="159" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="160" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="162" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="163" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="164" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="165" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="166" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="167" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="168" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="169" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="170" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="171" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="172" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="173" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="174" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="175" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="176" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="177" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="178" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="179" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="180" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="181" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="182" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="183" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="184" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="185" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="186" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="187" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="188" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="189" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="190" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="191" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="192" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="193" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="194" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="195" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="196" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="197" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="198" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="199" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="200" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="201" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="202" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="203" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="204" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="205" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="206" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="207" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="208" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="209" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="210" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="211" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="212" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="213" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="214" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="215" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="216" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="217" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="218" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="219" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="220" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="221" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="222" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="223" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="224" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="225" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="226" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="227" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="228" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="229" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="230" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="231" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="232" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="233" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="234" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="235" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="236" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="237" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="238" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="239" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="240" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="241" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="242" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="243" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="244" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="245" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="246" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="247" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="248" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="249" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="250" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="251" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="252" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="253" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="254" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="255" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="256" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="257" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="258" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="259" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="260" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="261" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="262" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="263" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="264" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="265" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="266" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="267" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="268" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="269" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="270" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="271" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="272" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="273" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="274" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="275" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="276" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="277" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="278" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="279" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="280" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="281" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="282" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="283" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="284" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="285" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="286" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="287" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="288" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="289" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="290" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="291" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="292" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="293" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="294" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="295" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="296" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="297" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="298" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="299" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="300" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="301" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="302" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="303" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="304" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="305" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="306" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="307" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="308" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="309" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="310" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="311" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="312" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="313" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="314" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="315" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="316" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="317" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="318" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="319" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="320" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="321" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="322" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="323" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="324" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="325" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="326" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="327" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="328" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="329" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="330" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="331" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="332" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="333" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="334" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="335" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="336" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="337" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="338" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="339" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="340" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="341" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="342" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="343" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="344" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="345" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="346" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="347" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="348" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="349" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="350" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="351" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="352" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="353" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="354" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="355" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="356" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="357" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="358" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="359" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="360" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="361" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="362" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="363" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="364" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="365" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="366" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="367" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="368" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="369" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="370" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="371" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="372" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="373" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="374" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="375" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="376" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="377" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="378" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="379" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="380" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="381" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="382" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="383" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="384" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="385" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="386" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="387" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="388" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="389" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="390" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="391" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="392" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="393" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="394" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="395" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="396" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="397" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="398" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="399" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="400" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="401" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="402" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="403" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="404" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="405" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="406" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="407" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="408" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="409" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="410" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="411" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="412" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="413" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="414" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="415" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="416" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A417"/>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A418"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -595,46 +915,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EB7AC2-4D9C-4E1E-B35E-489B916DA955}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -643,37 +935,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060541F5-E805-4846-A20F-B16F50AA258C}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A6:A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>